<commit_message>
not sure what changes
</commit_message>
<xml_diff>
--- a/static/img/ALL.Spring2018CourseOfferingGrid.xlsx
+++ b/static/img/ALL.Spring2018CourseOfferingGrid.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23240" windowHeight="15460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -4135,10 +4135,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="h:mm;@"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="h:mm;@"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="32" x14ac:knownFonts="1">
     <font>
@@ -4775,7 +4775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -4971,7 +4971,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5254,7 +5254,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -5406,7 +5406,7 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -5446,9 +5446,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="14" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="13" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="13" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -6101,7 +6101,7 @@
     <xf numFmtId="0" fontId="14" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -24131,9 +24131,9 @@
   </sheetPr>
   <dimension ref="A1:AL531"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A220" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M231" sqref="M231"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -24172,12 +24172,6 @@
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="318" t="s">
         <v>245</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C3" s="316">
-        <f>SUBTOTAL(3,C7:C510)</f>
-        <v>504</v>
       </c>
     </row>
     <row r="4" spans="1:38" s="324" customFormat="1" ht="56" x14ac:dyDescent="0.2">

</xml_diff>